<commit_message>
penambahan larangan sebelum print pada transaksi
</commit_message>
<xml_diff>
--- a/laporan/LaporanPenjualan.xlsx
+++ b/laporan/LaporanPenjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ade\test\project\laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C696DB9-2FE1-411B-98F4-F2464CC10B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B968323D-FB70-4994-A63F-657134CCD9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{CADD49E0-2809-4AC9-AB70-7099F97975ED}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{A67AEC56-0AB9-4DDE-B61D-EA875B341375}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>no_struk</t>
   </si>
@@ -172,6 +172,30 @@
   </si>
   <si>
     <t>Rp. 50,000</t>
+  </si>
+  <si>
+    <t>DK 5647 KM</t>
+  </si>
+  <si>
+    <t>Friday, July 2, 2021</t>
+  </si>
+  <si>
+    <t>DK 5678 HG</t>
+  </si>
+  <si>
+    <t>Wax, Engine</t>
+  </si>
+  <si>
+    <t>Rp. 230,000</t>
+  </si>
+  <si>
+    <t>Rp. 70,000</t>
+  </si>
+  <si>
+    <t>Rp. 80,000</t>
+  </si>
+  <si>
+    <t>Rp. 120,000</t>
   </si>
 </sst>
 </file>
@@ -522,8 +546,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783DF756-23EB-4A3E-A4DD-5207F15F7D34}">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D102BF-A1AF-45AB-AB1B-2A76D2BE5540}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -848,6 +872,90 @@
         <v>48</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12">
+        <v>200000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13">
+        <v>300000</v>
+      </c>
+      <c r="I13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>123</v>
+      </c>
+      <c r="B14">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14">
+        <v>200000</v>
+      </c>
+      <c r="I14" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>